<commit_message>
modified test data for census_employee_import
</commit_message>
<xml_diff>
--- a/spec/test_data/census_employee_import/DCHL Employee Census.xlsx
+++ b/spec/test_data/census_employee_import/DCHL Employee Census.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonioschaffert/workspace/ic/dc-enroll/spec/test_data/census_employee_import/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harsha/Desktop/ideacrew/enroll/spec/test_data/census_employee_import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664D52CB-463B-3F4C-B936-A17AD3F41D6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42B78AF-E548-0845-BE88-387C7C5BD1C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="488" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="14180" tabRatio="488" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Census" sheetId="6" r:id="rId1"/>
@@ -1429,9 +1429,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q5" sqref="Q5"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1628,7 +1628,7 @@
         <v>46</v>
       </c>
       <c r="H4" s="2">
-        <v>67867867</v>
+        <v>678678678</v>
       </c>
       <c r="I4" s="5">
         <v>32123</v>

</xml_diff>

<commit_message>
parsing ssn in census employee upload and display correct row number (#2734)
* passing ssn in census employee upload and display correct row number

* rubocop fix

* modified test data for census_employee_import

* spec fix
</commit_message>
<xml_diff>
--- a/spec/test_data/census_employee_import/DCHL Employee Census.xlsx
+++ b/spec/test_data/census_employee_import/DCHL Employee Census.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antonioschaffert/workspace/ic/dc-enroll/spec/test_data/census_employee_import/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harsha/Desktop/ideacrew/enroll/spec/test_data/census_employee_import/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664D52CB-463B-3F4C-B936-A17AD3F41D6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42B78AF-E548-0845-BE88-387C7C5BD1C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" tabRatio="488" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="25600" windowHeight="14180" tabRatio="488" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Census" sheetId="6" r:id="rId1"/>
@@ -1429,9 +1429,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q5" sqref="Q5"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1628,7 +1628,7 @@
         <v>46</v>
       </c>
       <c r="H4" s="2">
-        <v>67867867</v>
+        <v>678678678</v>
       </c>
       <c r="I4" s="5">
         <v>32123</v>

</xml_diff>